<commit_message>
add alternate source for SARB database
</commit_message>
<xml_diff>
--- a/data-raw/data-out/CAN-SAR_data_dictionary.xlsx
+++ b/data-raw/data-out/CAN-SAR_data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10128"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="7968"/>
   </bookViews>
   <sheets>
     <sheet name="Database Fields" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="491">
   <si>
     <t>Column header</t>
   </si>
@@ -1791,9 +1791,6 @@
     <t>Date that the species was added to SARA Schedule 1</t>
   </si>
   <si>
-    <t>Extracted from SAR Data Management System under 'Legal List'</t>
-  </si>
-  <si>
     <t>Outreach and stewardship</t>
   </si>
   <si>
@@ -1989,9 +1986,6 @@
     <t>Provinces, territories or oceans where the species is present</t>
   </si>
   <si>
-    <t>Extracted from SAR Data Management System under 'Legal List' or from the status report</t>
-  </si>
-  <si>
     <t>NA if not a status report</t>
   </si>
   <si>
@@ -2284,6 +2278,31 @@
   </si>
   <si>
     <t>Date that the Governor in Council amended SARA Schedule 1 to incorporate the species</t>
+  </si>
+  <si>
+    <t>Extracted from SARB (Species at Risk Branch) database under 'Legal List' or from the status report</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under Last assessment date)</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under Date added)</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under Last minister's receipt date)</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List' (Can also be found in the Response Statement, available on the SAR Public Registry Species Profile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracted from the SARB database under 'Legal List' ( Can also be found in the Order Acknowledging Receipt of the Assessment Done Pursuant to Subsection 23(1) of the Act, available on the SAR Public Registry Species Profile)
+</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List'  ( Can also be found in the Order Amending Schedules 1 to 3 to the Species at Risk Act, available on the SAR Public Registry Species Profile)</t>
+  </si>
+  <si>
+    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under GIC Decision)</t>
   </si>
 </sst>
 </file>
@@ -2568,11 +2587,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2986,8 +3005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3004,7 +3023,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="72">
       <c r="A1" s="34" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3034,13 +3053,13 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>19</v>
@@ -3059,13 +3078,13 @@
     </row>
     <row r="4" spans="1:15" ht="28.8">
       <c r="A4" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>19</v>
@@ -3090,7 +3109,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>4</v>
@@ -3115,7 +3134,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>4</v>
@@ -3134,22 +3153,22 @@
     </row>
     <row r="7" spans="1:15" ht="28.8">
       <c r="A7" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="D7" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="F7" s="26" t="s">
         <v>367</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>368</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -3166,10 +3185,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>8</v>
@@ -3192,13 +3211,13 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>371</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>372</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -3215,10 +3234,10 @@
     </row>
     <row r="10" spans="1:15" ht="43.2">
       <c r="A10" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="25" t="s">
@@ -3238,16 +3257,16 @@
     </row>
     <row r="11" spans="1:15" ht="28.8">
       <c r="A11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>375</v>
-      </c>
       <c r="D11" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -3263,13 +3282,13 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>7</v>
@@ -3288,16 +3307,16 @@
     </row>
     <row r="13" spans="1:15" ht="28.8">
       <c r="A13" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -3313,10 +3332,10 @@
     </row>
     <row r="14" spans="1:15" ht="28.8">
       <c r="A14" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="25" t="s">
@@ -3332,13 +3351,13 @@
     </row>
     <row r="15" spans="1:15" ht="43.2">
       <c r="A15" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>13</v>
@@ -3357,13 +3376,13 @@
     </row>
     <row r="16" spans="1:15" ht="28.8">
       <c r="A16" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>13</v>
@@ -3382,55 +3401,55 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="25" t="s">
+        <v>462</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="G17" s="25" t="s">
         <v>465</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="H17" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="I17" s="25" t="s">
         <v>467</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="J17" s="25" t="s">
         <v>468</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="K17" s="25" t="s">
         <v>469</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="L17" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="M17" s="25" t="s">
         <v>471</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="N17" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="O17" s="25" t="s">
         <v>473</v>
-      </c>
-      <c r="N17" s="25" t="s">
-        <v>474</v>
-      </c>
-      <c r="O17" s="25" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="28.8">
       <c r="A18" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>69</v>
@@ -3439,7 +3458,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
@@ -3468,7 +3487,7 @@
         <v>60</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -3499,7 +3518,7 @@
         <v>60</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
@@ -3528,7 +3547,7 @@
         <v>60</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -3554,7 +3573,7 @@
         <v>13</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="25"/>
@@ -3581,7 +3600,7 @@
         <v>13</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="25"/>
@@ -3608,7 +3627,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="25"/>
@@ -3623,10 +3642,10 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C25" s="29" t="s">
         <v>318</v>
@@ -3647,7 +3666,7 @@
         <v>118</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -3657,16 +3676,16 @@
     </row>
     <row r="26" spans="1:17" ht="72">
       <c r="A26" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>386</v>
+        <v>483</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I26" s="25"/>
       <c r="K26" s="25"/>
@@ -3677,19 +3696,19 @@
     </row>
     <row r="27" spans="1:17" ht="57.6">
       <c r="A27" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>320</v>
+        <v>484</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
@@ -3704,19 +3723,19 @@
     </row>
     <row r="28" spans="1:17" ht="57.6">
       <c r="A28" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>319</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>320</v>
+        <v>485</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
@@ -3731,19 +3750,19 @@
     </row>
     <row r="29" spans="1:17" ht="57.6">
       <c r="A29" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>320</v>
+        <v>486</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
@@ -3758,19 +3777,19 @@
     </row>
     <row r="30" spans="1:17" ht="57.6">
       <c r="A30" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>320</v>
+        <v>487</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
@@ -3783,21 +3802,21 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:17" ht="57.6">
+    <row r="31" spans="1:17" ht="72">
       <c r="A31" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>320</v>
+        <v>488</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
@@ -3812,19 +3831,19 @@
     </row>
     <row r="32" spans="1:17" ht="57.6">
       <c r="A32" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
@@ -3839,28 +3858,28 @@
     </row>
     <row r="33" spans="1:15" ht="57.6">
       <c r="A33" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>320</v>
+        <v>490</v>
       </c>
       <c r="D33" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="F33" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="G33" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="F33" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="G33" s="25" t="s">
-        <v>394</v>
-      </c>
       <c r="H33" s="27" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
@@ -3877,13 +3896,13 @@
         <v>68</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>73</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
@@ -3898,10 +3917,10 @@
     </row>
     <row r="35" spans="1:15" ht="57.6">
       <c r="A35" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>109</v>
@@ -3910,7 +3929,7 @@
         <v>110</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
@@ -3919,13 +3938,13 @@
     </row>
     <row r="36" spans="1:15" ht="57.6">
       <c r="A36" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
@@ -3946,7 +3965,7 @@
         <v>13</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
@@ -3955,19 +3974,19 @@
     </row>
     <row r="38" spans="1:15" ht="43.2">
       <c r="A38" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>110</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
@@ -3976,13 +3995,13 @@
     </row>
     <row r="39" spans="1:15" ht="57.6">
       <c r="A39" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
@@ -3997,13 +4016,13 @@
         <v>108</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>110</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
@@ -4024,13 +4043,13 @@
         <v>112</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>110</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
@@ -4048,10 +4067,10 @@
         <v>27</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>13</v>
@@ -4076,7 +4095,7 @@
         <v>62</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>13</v>
@@ -4095,13 +4114,13 @@
     </row>
     <row r="44" spans="1:15" ht="58.2" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B44" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>419</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>421</v>
       </c>
       <c r="D44" s="27">
         <v>0</v>
@@ -4110,10 +4129,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H44" s="25"/>
       <c r="I44" s="25"/>
@@ -4125,13 +4144,13 @@
     </row>
     <row r="45" spans="1:15" ht="101.4" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -4140,10 +4159,10 @@
         <v>1</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H45" s="26"/>
       <c r="I45" s="25"/>
@@ -4155,13 +4174,13 @@
     </row>
     <row r="46" spans="1:15" ht="101.4" thickBot="1">
       <c r="A46" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -4170,10 +4189,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -4185,13 +4204,13 @@
     </row>
     <row r="47" spans="1:15" ht="101.4" thickBot="1">
       <c r="A47" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D47" s="27">
         <v>0</v>
@@ -4200,21 +4219,21 @@
         <v>1</v>
       </c>
       <c r="F47" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="101.4" thickBot="1">
       <c r="A48" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D48" s="27">
         <v>0</v>
@@ -4223,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="F48" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="187.2">
@@ -4237,7 +4256,7 @@
         <v>63</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>13</v>
@@ -4253,7 +4272,7 @@
         <v>116</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D50" s="26" t="s">
         <v>117</v>
@@ -4266,7 +4285,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>13</v>
@@ -4277,13 +4296,13 @@
     </row>
     <row r="52" spans="1:16" ht="72">
       <c r="A52" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D52" s="1">
         <v>1.1000000000000001</v>
@@ -4292,7 +4311,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -4306,19 +4325,19 @@
     </row>
     <row r="53" spans="1:16" ht="28.8">
       <c r="A53" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G53" s="1"/>
       <c r="I53" s="1"/>
@@ -4332,19 +4351,19 @@
     </row>
     <row r="54" spans="1:16" ht="28.8">
       <c r="A54" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -4359,19 +4378,19 @@
     </row>
     <row r="55" spans="1:16" ht="28.8">
       <c r="A55" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G55" s="1"/>
       <c r="I55" s="1"/>
@@ -4384,31 +4403,31 @@
     </row>
     <row r="56" spans="1:16" ht="28.8">
       <c r="A56" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>413</v>
-      </c>
       <c r="I56" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J56" s="26"/>
       <c r="K56" s="26"/>
@@ -4419,31 +4438,31 @@
     </row>
     <row r="57" spans="1:16" ht="28.8">
       <c r="A57" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="F57" s="24" t="s">
+      <c r="H57" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="H57" s="24" t="s">
-        <v>413</v>
-      </c>
       <c r="I57" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J57" s="26"/>
       <c r="K57" s="26"/>
@@ -4454,19 +4473,19 @@
     </row>
     <row r="58" spans="1:16" ht="28.8">
       <c r="A58" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -4481,19 +4500,19 @@
     </row>
     <row r="59" spans="1:16" ht="28.8">
       <c r="A59" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G59" s="1"/>
       <c r="I59" s="1"/>
@@ -4509,10 +4528,10 @@
         <v>121</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>13</v>
@@ -4531,13 +4550,13 @@
     </row>
     <row r="61" spans="1:16" ht="158.4">
       <c r="A61" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D61" s="24">
         <v>0</v>
@@ -4566,10 +4585,10 @@
         <v>64</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>29</v>
@@ -4590,13 +4609,13 @@
         <v>34</v>
       </c>
       <c r="K62" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="L62" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="M62" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="L62" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="N62" s="25"/>
       <c r="O62" s="25"/>
@@ -4609,10 +4628,10 @@
         <v>65</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>35</v>
@@ -4633,13 +4652,13 @@
         <v>34</v>
       </c>
       <c r="K63" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="L63" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="M63" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="L63" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="N63" s="25"/>
       <c r="O63" s="25"/>
@@ -4652,10 +4671,10 @@
         <v>66</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>40</v>
@@ -4676,13 +4695,13 @@
         <v>45</v>
       </c>
       <c r="K64" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="L64" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="M64" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="L64" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="N64" s="25"/>
       <c r="O64" s="25"/>
@@ -4695,10 +4714,10 @@
         <v>67</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>46</v>
@@ -4716,13 +4735,13 @@
         <v>50</v>
       </c>
       <c r="J65" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="K65" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="K65" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="L65" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="M65" s="25"/>
       <c r="N65" s="25"/>
@@ -4730,36 +4749,36 @@
     </row>
     <row r="66" spans="1:15" ht="28.8">
       <c r="A66" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>449</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="B66" s="24" t="s">
-        <v>451</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="D66" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="43.2">
       <c r="A67" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D67" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -4771,7 +4790,7 @@
       <formula>C24&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49 B20:C20 B4:C4 B27:C32 B64:C65 C50 B60:C62 B12:C18 C19:C23 C25:C26 C28:C33 C63:C65 C5:C12 C3">
+  <conditionalFormatting sqref="B49 B20:C20 B4:C4 B27:C32 B64:C65 C50 B60:C62 B12:C18 C19:C23 C25:C26 C63:C65 C5:C12 C3 C28:C33">
     <cfRule type="expression" dxfId="14" priority="23">
       <formula>B3&lt;&gt;#REF!</formula>
     </cfRule>
@@ -4879,24 +4898,24 @@
     </row>
     <row r="2" spans="1:3" ht="43.2">
       <c r="A2" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8">
       <c r="A3" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" customHeight="1">
@@ -4907,7 +4926,7 @@
         <v>81</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58.2" customHeight="1">
@@ -4918,7 +4937,7 @@
         <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2">
@@ -4981,7 +5000,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>94</v>
@@ -5205,11 +5224,11 @@
       <c r="Y4" s="6"/>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="13" t="s">
         <v>130</v>
       </c>
@@ -5424,11 +5443,11 @@
       <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="13" t="s">
         <v>145</v>
       </c>
@@ -5703,11 +5722,11 @@
       <c r="Y20" s="6"/>
     </row>
     <row r="21" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="13" t="s">
         <v>163</v>
       </c>
@@ -5922,11 +5941,11 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="13" t="s">
         <v>178</v>
       </c>
@@ -6203,11 +6222,11 @@
       <c r="Y36" s="6"/>
     </row>
     <row r="37" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="13" t="s">
         <v>197</v>
       </c>
@@ -6484,11 +6503,11 @@
       <c r="Y45" s="6"/>
     </row>
     <row r="46" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="13" t="s">
         <v>216</v>
       </c>
@@ -6703,11 +6722,11 @@
       <c r="Y52" s="6"/>
     </row>
     <row r="53" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="13" t="s">
         <v>231</v>
       </c>
@@ -6920,11 +6939,11 @@
       <c r="Y59" s="6"/>
     </row>
     <row r="60" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="40" t="s">
         <v>244</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
       <c r="D60" s="13" t="s">
         <v>245</v>
       </c>
@@ -7139,11 +7158,11 @@
       <c r="Y66" s="6"/>
     </row>
     <row r="67" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="42"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
       <c r="D67" s="13" t="s">
         <v>260</v>
       </c>
@@ -7544,11 +7563,11 @@
       <c r="Y79" s="6"/>
     </row>
     <row r="80" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="13" t="s">
         <v>287</v>
       </c>
@@ -7757,11 +7776,11 @@
       <c r="Y86" s="6"/>
     </row>
     <row r="87" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A87" s="41" t="s">
+      <c r="A87" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="B87" s="42"/>
-      <c r="C87" s="42"/>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
       <c r="D87" s="13" t="s">
         <v>299</v>
       </c>
@@ -8008,8 +8027,8 @@
       <c r="C95" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="D95" s="40"/>
-      <c r="E95" s="40"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -14138,6 +14157,123 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
@@ -14152,123 +14288,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>

<commit_message>
update to ECCC internal database
</commit_message>
<xml_diff>
--- a/data-raw/data-out/CAN-SAR_data_dictionary.xlsx
+++ b/data-raw/data-out/CAN-SAR_data_dictionary.xlsx
@@ -2010,9 +2010,6 @@
     <t>NA if not a recovery strategy</t>
   </si>
   <si>
-    <t>Based on the critical habitat section of the Recovery Strategy. If critical habitat is described as fully identified or identified to the extent possible then a 'Y' was recorded. If critical habitat was described as partially identified then a 'P' was recorded. If critical habitat was not identified then an 'N' was recorded and if thethe document is not a Recovery Strategy then NA was recorded</t>
-  </si>
-  <si>
     <t>Whether an "IUCN Threats Assessment" was included in the document</t>
   </si>
   <si>
@@ -2256,16 +2253,19 @@
     <t>Note that "NE" means Not Extracted throughout the database and indicates that the data has not been extracted but could be</t>
   </si>
   <si>
-    <t>Extracted from SARB (Species at Risk Branch) database under 'Legal List' or from the status report</t>
-  </si>
-  <si>
-    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under Last assessment date)</t>
-  </si>
-  <si>
-    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under Date added)</t>
-  </si>
-  <si>
-    <t>Extracted from the SARB database under 'Legal List' (Can also be found on the SAR Public Registry Species Profile under GIC Decision)</t>
+    <t>Based on the critical habitat section of the Recovery Strategy. If critical habitat is described as fully identified or identified to the extent possible then a 'Y' was recorded. If critical habitat was described as partially identified then a 'P' was recorded. If critical habitat was not identified then an 'N' was recorded and if the document is not a Recovery Strategy then NA was recorded</t>
+  </si>
+  <si>
+    <t>Extracted from an ECCC internal database (Can also be found on the SAR Public Registry Species Profile under Last assessment date)</t>
+  </si>
+  <si>
+    <t>Extracted from an ECCC internal database (Can also be found on the SAR Public Registry Species Profile under Date added)</t>
+  </si>
+  <si>
+    <t>Extracted from an ECCC internal database (Can also be found on the SAR Public Registry Species Profile under GIC Decision)</t>
+  </si>
+  <si>
+    <t>Extracted from an ECCC internal database or from the status report</t>
   </si>
 </sst>
 </file>
@@ -2550,11 +2550,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2968,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2986,7 +2986,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="72">
       <c r="A1" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3016,13 +3016,13 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B3" s="27" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>19</v>
@@ -3041,13 +3041,13 @@
     </row>
     <row r="4" spans="1:15" ht="28.8">
       <c r="A4" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>19</v>
@@ -3072,7 +3072,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>4</v>
@@ -3097,7 +3097,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>4</v>
@@ -3148,10 +3148,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>470</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>471</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>8</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="10" spans="1:15" ht="43.2">
       <c r="A10" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>472</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>473</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="25" t="s">
@@ -3276,7 +3276,7 @@
         <v>371</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>366</v>
@@ -3364,55 +3364,55 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="25" t="s">
+        <v>455</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>456</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="F17" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="G17" s="25" t="s">
         <v>458</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="H17" s="25" t="s">
         <v>459</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="I17" s="25" t="s">
         <v>460</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="J17" s="25" t="s">
         <v>461</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="K17" s="25" t="s">
         <v>462</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="L17" s="25" t="s">
         <v>463</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="M17" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="N17" s="25" t="s">
         <v>465</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="O17" s="25" t="s">
         <v>466</v>
-      </c>
-      <c r="O17" s="25" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="28.8">
       <c r="A18" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>67</v>
@@ -3645,7 +3645,7 @@
         <v>378</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>377</v>
@@ -3665,7 +3665,7 @@
         <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D27" s="27" t="s">
         <v>366</v>
@@ -3692,7 +3692,7 @@
         <v>317</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>366</v>
@@ -3719,7 +3719,7 @@
         <v>387</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>383</v>
@@ -3734,7 +3734,7 @@
         <v>386</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
@@ -3751,7 +3751,7 @@
         <v>66</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>393</v>
+        <v>474</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>71</v>
@@ -3922,10 +3922,10 @@
         <v>27</v>
       </c>
       <c r="B38" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="C38" s="27" t="s">
         <v>395</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>396</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>13</v>
@@ -3950,7 +3950,7 @@
         <v>60</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>13</v>
@@ -3972,10 +3972,10 @@
         <v>346</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D40" s="27">
         <v>0</v>
@@ -3987,7 +3987,7 @@
         <v>382</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
@@ -4002,10 +4002,10 @@
         <v>347</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D41" s="27">
         <v>0</v>
@@ -4017,7 +4017,7 @@
         <v>382</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H41" s="26"/>
       <c r="I41" s="25"/>
@@ -4032,10 +4032,10 @@
         <v>348</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D42" s="27">
         <v>0</v>
@@ -4047,7 +4047,7 @@
         <v>382</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
@@ -4062,10 +4062,10 @@
         <v>349</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D43" s="27">
         <v>0</v>
@@ -4077,7 +4077,7 @@
         <v>382</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="101.4" thickBot="1">
@@ -4085,10 +4085,10 @@
         <v>350</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D44" s="27">
         <v>0</v>
@@ -4100,7 +4100,7 @@
         <v>382</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="187.2">
@@ -4111,7 +4111,7 @@
         <v>61</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>13</v>
@@ -4127,7 +4127,7 @@
         <v>114</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D46" s="26" t="s">
         <v>115</v>
@@ -4140,7 +4140,7 @@
         <v>26</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>13</v>
@@ -4154,10 +4154,10 @@
         <v>351</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D48" s="1">
         <v>1.1000000000000001</v>
@@ -4166,7 +4166,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -4183,16 +4183,16 @@
         <v>352</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>366</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G49" s="1"/>
       <c r="I49" s="1"/>
@@ -4209,16 +4209,16 @@
         <v>353</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -4236,16 +4236,16 @@
         <v>354</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G51" s="1"/>
       <c r="I51" s="1"/>
@@ -4261,28 +4261,28 @@
         <v>355</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>405</v>
-      </c>
       <c r="I52" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J52" s="26"/>
       <c r="K52" s="26"/>
@@ -4296,28 +4296,28 @@
         <v>356</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F53" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="F53" s="24" t="s">
+      <c r="G53" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="H53" s="24" t="s">
-        <v>405</v>
-      </c>
       <c r="I53" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="26"/>
@@ -4331,16 +4331,16 @@
         <v>357</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -4358,16 +4358,16 @@
         <v>358</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G55" s="1"/>
       <c r="I55" s="1"/>
@@ -4383,10 +4383,10 @@
         <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>13</v>
@@ -4405,13 +4405,13 @@
     </row>
     <row r="57" spans="1:16" ht="158.4">
       <c r="A57" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>424</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -4440,10 +4440,10 @@
         <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>29</v>
@@ -4464,13 +4464,13 @@
         <v>34</v>
       </c>
       <c r="K58" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="L58" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="L58" s="33" t="s">
+      <c r="M58" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="N58" s="25"/>
       <c r="O58" s="25"/>
@@ -4483,10 +4483,10 @@
         <v>63</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>35</v>
@@ -4507,13 +4507,13 @@
         <v>34</v>
       </c>
       <c r="K59" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="L59" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="L59" s="33" t="s">
+      <c r="M59" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="N59" s="25"/>
       <c r="O59" s="25"/>
@@ -4526,10 +4526,10 @@
         <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>40</v>
@@ -4550,13 +4550,13 @@
         <v>45</v>
       </c>
       <c r="K60" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="L60" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="L60" s="33" t="s">
+      <c r="M60" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
@@ -4569,10 +4569,10 @@
         <v>65</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>46</v>
@@ -4590,13 +4590,13 @@
         <v>50</v>
       </c>
       <c r="J61" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="K61" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="K61" s="33" t="s">
+      <c r="L61" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="M61" s="25"/>
       <c r="N61" s="25"/>
@@ -4604,36 +4604,36 @@
     </row>
     <row r="62" spans="1:16" ht="28.8">
       <c r="A62" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B62" s="24" t="s">
         <v>442</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="C62" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="43.2">
       <c r="A63" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>449</v>
+      </c>
+      <c r="C63" s="24" t="s">
         <v>447</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>448</v>
       </c>
       <c r="D63" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -5079,11 +5079,11 @@
       <c r="Y4" s="6"/>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="13" t="s">
         <v>128</v>
       </c>
@@ -5298,11 +5298,11 @@
       <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="13" t="s">
         <v>143</v>
       </c>
@@ -5577,11 +5577,11 @@
       <c r="Y20" s="6"/>
     </row>
     <row r="21" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="13" t="s">
         <v>161</v>
       </c>
@@ -5796,11 +5796,11 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="13" t="s">
         <v>176</v>
       </c>
@@ -6077,11 +6077,11 @@
       <c r="Y36" s="6"/>
     </row>
     <row r="37" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="13" t="s">
         <v>195</v>
       </c>
@@ -6358,11 +6358,11 @@
       <c r="Y45" s="6"/>
     </row>
     <row r="46" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="13" t="s">
         <v>214</v>
       </c>
@@ -6577,11 +6577,11 @@
       <c r="Y52" s="6"/>
     </row>
     <row r="53" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="13" t="s">
         <v>229</v>
       </c>
@@ -6794,11 +6794,11 @@
       <c r="Y59" s="6"/>
     </row>
     <row r="60" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
       <c r="D60" s="13" t="s">
         <v>243</v>
       </c>
@@ -7013,11 +7013,11 @@
       <c r="Y66" s="6"/>
     </row>
     <row r="67" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="C67" s="42"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
       <c r="D67" s="13" t="s">
         <v>258</v>
       </c>
@@ -7418,11 +7418,11 @@
       <c r="Y79" s="6"/>
     </row>
     <row r="80" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="13" t="s">
         <v>285</v>
       </c>
@@ -7631,11 +7631,11 @@
       <c r="Y86" s="6"/>
     </row>
     <row r="87" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A87" s="41" t="s">
+      <c r="A87" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="B87" s="42"/>
-      <c r="C87" s="42"/>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
       <c r="D87" s="13" t="s">
         <v>297</v>
       </c>
@@ -7882,8 +7882,8 @@
       <c r="C95" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="D95" s="40"/>
-      <c r="E95" s="40"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -14012,6 +14012,123 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
@@ -14026,123 +14143,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>